<commit_message>
MSAA Enable and update rubric
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -336,6 +336,49 @@
   </si>
   <si>
     <t>I</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.braynzarsoft.net/</t>
+  </si>
+  <si>
+    <t>3D Game Programming with DirectX 11</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -861,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -981,14 +1024,16 @@
       <c r="E4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="G4" s="8">
         <f t="shared" ref="G4:G35" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H4" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
@@ -1000,11 +1045,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1023,10 +1068,12 @@
       <c r="E5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1063,7 +1110,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1131,15 +1178,15 @@
       </c>
       <c r="H8" s="10">
         <f>H4+IF(H4 &lt; 22, IF(K4+H4 &gt; 22, 22- H4, K4),0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I8" s="9">
         <f>I4+IF(I4 &lt; 22, IF(H10+I4 &gt; 22, 22- I4, H10),0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1196,11 +1243,11 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -1354,10 +1401,12 @@
       <c r="E18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1481,10 +1530,12 @@
       <c r="E23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G23" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1620,10 +1671,12 @@
       <c r="E30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G30" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1647,10 +1700,12 @@
       <c r="E31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G31" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -1674,10 +1729,12 @@
       <c r="E32" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G32" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -1701,10 +1758,12 @@
       <c r="E33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -2151,11 +2210,15 @@
       <c r="D54" s="5">
         <v>3</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="3"/>
+      <c r="E54" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G54" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -2176,11 +2239,15 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="E55" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2831,7 +2898,9 @@
       <c r="B90" s="6">
         <v>3</v>
       </c>
-      <c r="C90" s="3"/>
+      <c r="C90" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
@@ -2849,7 +2918,9 @@
       <c r="B91" s="6">
         <v>1</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
@@ -2894,10 +2965,14 @@
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A95" s="16"/>
+      <c r="A95" s="16" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A96" s="16"/>
+      <c r="A96" s="16" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" s="16"/>
@@ -2985,7 +3060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
bumping map work but lighting weird
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -375,6 +375,22 @@
   </si>
   <si>
     <t>3D Game Programming with DirectX 11</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -904,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1045,11 +1061,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1110,7 +1126,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1186,7 +1202,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1243,11 +1259,11 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -2439,11 +2455,15 @@
       <c r="D65" s="5">
         <v>2</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="3"/>
+      <c r="E65" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="G65" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -2464,11 +2484,15 @@
       <c r="D66" s="5">
         <v>3</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="3"/>
+      <c r="E66" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="G66" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
@@ -3060,7 +3084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Save for rewrite lighting stuff
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -415,6 +415,10 @@
   </si>
   <si>
     <t>I</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>II</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -952,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1189,7 +1193,9 @@
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
@@ -3134,7 +3140,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Update rubric and move the other two lighting algorithms to separate  function
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -431,6 +431,14 @@
   </si>
   <si>
     <t>II</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -956,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1097,11 +1105,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1164,7 +1172,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1242,7 +1250,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1299,11 +1307,11 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
@@ -2006,11 +2014,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="G40" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -3140,7 +3152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Three lighting work. Known issue: Flashlight not apply to the fking barrel
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -426,19 +426,15 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>II</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>II</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>I</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -964,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1105,11 +1101,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1172,7 +1168,7 @@
       </c>
       <c r="H6" s="5">
         <f>IF(SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91)  &gt; 22, SUMIF(E4:E85,"=I",G4:G85) + SUMIF(C90:C91, "X",B90:B91) - 22,0)</f>
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
@@ -1185,7 +1181,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
@@ -1202,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="8">
@@ -1250,7 +1246,7 @@
       </c>
       <c r="J8" s="9">
         <f>J4+IF(J4 &lt; 22, IF(I10+J4 &gt; 22, 22- J4, I10),0)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1307,15 +1303,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1855,12 +1851,14 @@
         <v>1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F34" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G34" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -1882,12 +1880,14 @@
         <v>1</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F35" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G35" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -1909,12 +1909,14 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G36" s="8">
         <f t="shared" ref="G36:G67" si="1" xml:space="preserve"> IF(EXACT(F36,"X"),IF(EXACT(E36,"I"),$B36,IF(EXACT(E36,"II"),$C36,IF(EXACT(E36,"III"),$D36,0))),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
@@ -2015,10 +2017,10 @@
         <v>3</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G40" s="8">
         <f t="shared" si="1"/>
@@ -3152,7 +3154,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Put three optional shaders runtime compiling function in to the D3DUtils
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -473,6 +473,42 @@
   </si>
   <si>
     <t>II</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -1017,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1150,19 +1186,19 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>87</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1231,16 +1267,16 @@
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
@@ -1287,11 +1323,15 @@
       <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8" s="10">
         <f>H4+IF(H4 &lt; 22, IF(K4+H4 &gt; 22, 22- H4, K4),0)</f>
@@ -1360,15 +1400,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1544,11 +1584,15 @@
       <c r="D19" s="5">
         <v>3</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="G19" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1594,11 +1638,15 @@
       <c r="D21" s="5">
         <v>3</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -2021,11 +2069,15 @@
       <c r="D38" s="5">
         <v>3</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="G38" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
@@ -2224,11 +2276,15 @@
       <c r="D47" s="5">
         <v>5</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="3"/>
+      <c r="E47" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="G47" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -3060,8 +3116,12 @@
       <c r="C90" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
@@ -3080,8 +3140,12 @@
       <c r="C91" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3219,7 +3283,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Create Camera class, pending for refine code structures
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="116">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -428,10 +428,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>II</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -440,10 +436,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>II</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>I</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -460,10 +452,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>II</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -472,10 +460,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>II</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -513,6 +497,14 @@
   </si>
   <si>
     <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1053,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1186,7 +1178,7 @@
       </c>
       <c r="I4" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91))</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="J4" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91))</f>
@@ -1194,7 +1186,7 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
@@ -1252,10 +1244,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G6" s="8">
         <f t="shared" si="0"/>
@@ -1267,11 +1259,11 @@
       </c>
       <c r="I6" s="5">
         <f>IF(SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=II",G4:G85) + SUMIF(D90:D91, "X",B90:B91) - 22,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="9">
@@ -1324,10 +1316,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
@@ -1400,7 +1392,7 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
@@ -1585,10 +1577,10 @@
         <v>3</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="0"/>
@@ -1639,10 +1631,10 @@
         <v>3</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
@@ -1668,10 +1660,10 @@
         <v>3</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" si="0"/>
@@ -1726,10 +1718,10 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
@@ -2016,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>81</v>
@@ -2070,10 +2062,10 @@
         <v>3</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G38" s="8">
         <f t="shared" si="1"/>
@@ -2128,10 +2120,10 @@
         <v>3</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G40" s="8">
         <f t="shared" si="1"/>
@@ -2277,10 +2269,10 @@
         <v>5</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G47" s="8">
         <f t="shared" si="1"/>
@@ -2468,10 +2460,10 @@
         <v>5</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G56" s="8">
         <f t="shared" si="1"/>
@@ -2726,10 +2718,10 @@
         <v>5</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G68" s="8">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
@@ -3283,7 +3275,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
tessellation terrain not working...
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -35,6 +35,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="F46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+The mirror does reject rendering the object that being blocked. I don't know if this fulfill the requirement.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F56" authorId="0" shapeId="0">
       <text>
         <r>
@@ -66,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="119">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -505,6 +531,18 @@
   </si>
   <si>
     <t>III</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1045,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1186,11 +1224,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1263,12 +1301,12 @@
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
@@ -1284,11 +1322,15 @@
       <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="G7" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
@@ -1392,15 +1434,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2218,11 +2260,15 @@
       <c r="D45" s="5">
         <v>5</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3"/>
+      <c r="E45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="G45" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -2243,11 +2289,15 @@
       <c r="D46" s="5">
         <v>3</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="G46" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>

</xml_diff>

<commit_message>
Fix the tiled texturing for the terrain.
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -553,6 +553,18 @@
   </si>
   <si>
     <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>III</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -1097,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1238,11 +1250,11 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(H6,I6,J6)</f>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="L4" s="9">
         <f>SUM(G4:G85) + SUMIF(C90:C91, "X",B90:B91) + SUMIF(D90:D91, "X",B90:B91) + SUMIF(E90:E91, "X",B90:B91)</f>
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1315,12 +1327,12 @@
       </c>
       <c r="J6" s="5">
         <f>IF(SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) &gt; 22, SUMIF(E4:E85,"=III",G4:G85) + SUMIF(E90:E91, "X",B90:B91) - 22,0)</f>
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="9">
         <f>IF(L4 &gt; 66, SUM(-66,L4),0)</f>
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
@@ -1448,15 +1460,15 @@
       </c>
       <c r="H10" s="5">
         <f>IF(K4+H4 - 22 &gt; 0, K4+H4 - 22, 0)</f>
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="I10" s="5">
         <f>IF(H10+I4 - 22 &gt; 0, H10+I4 - 22, 0)</f>
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="J10" s="5">
         <f>IF(I10+J4 - 22 &gt; 0, I10+J4 - 22, 0)</f>
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -1664,12 +1676,10 @@
       <c r="E20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -2328,11 +2338,15 @@
       <c r="D47" s="5">
         <v>5</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="3"/>
+      <c r="E47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="G47" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2906,11 +2920,15 @@
       <c r="D75" s="5">
         <v>5</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="3"/>
+      <c r="E75" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="G75" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
@@ -3331,7 +3349,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Storm, Earth, and Fire! Hear my call!! (Particle system done)
</commit_message>
<xml_diff>
--- a/Documents & Instructions/Graphics II Project Rubric.xlsx
+++ b/Documents & Instructions/Graphics II Project Rubric.xlsx
@@ -32,32 +32,6 @@
             <charset val="1"/>
           </rPr>
           <t>Fill out name and repo address then submit to intial turn in on the graphics II sidekick.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>Chen Lu:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-The tesselation based on the LOD is sometime not working properly with no clue why causes that. Basicly the debug mode and release mode gave sometime different results or same results on different runs...</t>
         </r>
       </text>
     </comment>
@@ -1109,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>